<commit_message>
Add journal network analysis and new plots
</commit_message>
<xml_diff>
--- a/output/network_analysis_results.xlsx
+++ b/output/network_analysis_results.xlsx
@@ -350,6 +350,9 @@
     <t xml:space="preserve">Southern Asia</t>
   </si>
   <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
     <t xml:space="preserve">0000-0002-7613-1985</t>
   </si>
   <si>
@@ -399,9 +402,6 @@
   </si>
   <si>
     <t xml:space="preserve">0000-0002-9270-8860</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
   </si>
   <si>
     <t xml:space="preserve">0000-0001-9764-685X</t>
@@ -920,7 +920,7 @@
         <v>0.00561124396894327</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0138308060983979</v>
+        <v>0.013830806098398</v>
       </c>
       <c r="M2" t="n">
         <v>0.304030612244898</v>
@@ -988,7 +988,7 @@
         <v>0.0150983571463504</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0839331010108214</v>
+        <v>0.0839331010108216</v>
       </c>
       <c r="M3" t="n">
         <v>0.159544890115983</v>
@@ -1056,7 +1056,7 @@
         <v>0.00536040706874545</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0278381928086925</v>
+        <v>0.0278381928086926</v>
       </c>
       <c r="M4" t="n">
         <v>0.55780029296875</v>
@@ -1420,13 +1420,13 @@
         <v>0.666666666666667</v>
       </c>
       <c r="T9" t="n">
-        <v>0.420289855072464</v>
+        <v>0.442028985507246</v>
       </c>
       <c r="U9" t="n">
         <v>0.318840579710145</v>
       </c>
       <c r="V9" t="n">
-        <v>0.469979296066253</v>
+        <v>0.473084886128364</v>
       </c>
     </row>
     <row r="10">
@@ -1464,7 +1464,7 @@
         <v>0.00764009936812355</v>
       </c>
       <c r="L10" t="n">
-        <v>0.0349272449979199</v>
+        <v>0.03492724499792</v>
       </c>
       <c r="M10" t="n">
         <v>0.294365485338222</v>
@@ -1760,13 +1760,13 @@
         <v>0.905797101449275</v>
       </c>
       <c r="T14" t="n">
-        <v>0.884057971014493</v>
+        <v>0.91304347826087</v>
       </c>
       <c r="U14" t="n">
         <v>0.710144927536232</v>
       </c>
       <c r="V14" t="n">
-        <v>0.72463768115942</v>
+        <v>0.728778467908903</v>
       </c>
     </row>
     <row r="15">
@@ -1804,7 +1804,7 @@
         <v>0.0201789348486577</v>
       </c>
       <c r="L15" t="n">
-        <v>0.207572939006936</v>
+        <v>0.207572939006937</v>
       </c>
       <c r="M15" t="n">
         <v>0.12625761721303</v>
@@ -1896,13 +1896,13 @@
         <v>0.753623188405797</v>
       </c>
       <c r="T16" t="n">
-        <v>0.77536231884058</v>
+        <v>0.768115942028985</v>
       </c>
       <c r="U16" t="n">
         <v>0.855072463768116</v>
       </c>
       <c r="V16" t="n">
-        <v>0.778467908902692</v>
+        <v>0.777432712215321</v>
       </c>
     </row>
     <row r="17">
@@ -2008,7 +2008,7 @@
         <v>0.0151141118101966</v>
       </c>
       <c r="L18" t="n">
-        <v>0.167225455974456</v>
+        <v>0.167225455974457</v>
       </c>
       <c r="M18" t="n">
         <v>0.152885553106032</v>
@@ -2076,7 +2076,7 @@
         <v>0.00589037232752201</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0458282378778817</v>
+        <v>0.0458282378778818</v>
       </c>
       <c r="M19" t="n">
         <v>0.240692152375353</v>
@@ -2280,7 +2280,7 @@
         <v>0.0162899230162693</v>
       </c>
       <c r="L22" t="n">
-        <v>0.733009500122736</v>
+        <v>0.733009500122735</v>
       </c>
       <c r="M22" t="n">
         <v>0.112130346179756</v>
@@ -2348,7 +2348,7 @@
         <v>0.0175524456296892</v>
       </c>
       <c r="L23" t="n">
-        <v>0.791415183908864</v>
+        <v>0.791415183908863</v>
       </c>
       <c r="M23" t="n">
         <v>0.115402426110543</v>
@@ -2372,13 +2372,13 @@
         <v>0.72463768115942</v>
       </c>
       <c r="T23" t="n">
-        <v>0.77536231884058</v>
+        <v>0.753623188405797</v>
       </c>
       <c r="U23" t="n">
         <v>0.855072463768116</v>
       </c>
       <c r="V23" t="n">
-        <v>0.774327122153209</v>
+        <v>0.771221532091097</v>
       </c>
     </row>
     <row r="24">
@@ -2534,7 +2534,7 @@
         <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="G26" t="n">
         <v>10</v>
@@ -2620,7 +2620,7 @@
         <v>0.0175524456296892</v>
       </c>
       <c r="L27" t="n">
-        <v>0.791415183908863</v>
+        <v>0.791415183908864</v>
       </c>
       <c r="M27" t="n">
         <v>0.115402426110543</v>
@@ -2644,13 +2644,13 @@
         <v>0.739130434782609</v>
       </c>
       <c r="T27" t="n">
-        <v>0.753623188405797</v>
+        <v>0.782608695652174</v>
       </c>
       <c r="U27" t="n">
         <v>0.855072463768116</v>
       </c>
       <c r="V27" t="n">
-        <v>0.773291925465838</v>
+        <v>0.777432712215321</v>
       </c>
     </row>
     <row r="28">
@@ -2848,13 +2848,13 @@
         <v>0.565217391304348</v>
       </c>
       <c r="T30" t="n">
-        <v>0.797101449275362</v>
+        <v>0.811594202898551</v>
       </c>
       <c r="U30" t="n">
         <v>0.608695652173913</v>
       </c>
       <c r="V30" t="n">
-        <v>0.632505175983437</v>
+        <v>0.634575569358178</v>
       </c>
     </row>
     <row r="31">
@@ -2892,7 +2892,7 @@
         <v>0.0144064771370706</v>
       </c>
       <c r="L31" t="n">
-        <v>0.154358780575308</v>
+        <v>0.154358780575309</v>
       </c>
       <c r="M31" t="n">
         <v>0.148987950088056</v>
@@ -2960,7 +2960,7 @@
         <v>0.00827422605107342</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0717673158343308</v>
+        <v>0.0717673158343307</v>
       </c>
       <c r="M32" t="n">
         <v>0.209729237422045</v>
@@ -3052,13 +3052,13 @@
         <v>0.905797101449275</v>
       </c>
       <c r="T33" t="n">
-        <v>0.949275362318841</v>
+        <v>0.91304347826087</v>
       </c>
       <c r="U33" t="n">
         <v>0.710144927536232</v>
       </c>
       <c r="V33" t="n">
-        <v>0.733954451345756</v>
+        <v>0.728778467908903</v>
       </c>
     </row>
     <row r="34">
@@ -3078,7 +3078,7 @@
         <v>26</v>
       </c>
       <c r="F34" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="G34" t="n">
         <v>15</v>
@@ -3188,13 +3188,13 @@
         <v>0.818840579710145</v>
       </c>
       <c r="T35" t="n">
-        <v>0.949275362318841</v>
+        <v>0.978260869565217</v>
       </c>
       <c r="U35" t="n">
         <v>0.710144927536232</v>
       </c>
       <c r="V35" t="n">
-        <v>0.721532091097308</v>
+        <v>0.725672877846791</v>
       </c>
     </row>
     <row r="36">
@@ -3324,13 +3324,13 @@
         <v>0.818840579710145</v>
       </c>
       <c r="T37" t="n">
-        <v>0.905797101449275</v>
+        <v>0.91304347826087</v>
       </c>
       <c r="U37" t="n">
         <v>0.710144927536232</v>
       </c>
       <c r="V37" t="n">
-        <v>0.715320910973085</v>
+        <v>0.716356107660455</v>
       </c>
     </row>
     <row r="38">
@@ -3368,7 +3368,7 @@
         <v>0.00845880699654408</v>
       </c>
       <c r="L38" t="n">
-        <v>0.0583970592156716</v>
+        <v>0.0583970592156718</v>
       </c>
       <c r="M38" t="n">
         <v>0.417432720158376</v>
@@ -3504,7 +3504,7 @@
         <v>0.00845880699654408</v>
       </c>
       <c r="L40" t="n">
-        <v>0.0583970592156716</v>
+        <v>0.0583970592156718</v>
       </c>
       <c r="M40" t="n">
         <v>0.417432720158376</v>
@@ -3554,7 +3554,7 @@
         <v>110</v>
       </c>
       <c r="F41" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="G41" t="n">
         <v>12</v>
@@ -3572,7 +3572,7 @@
         <v>0.0096336631974354</v>
       </c>
       <c r="L41" t="n">
-        <v>0.0869317804477024</v>
+        <v>0.0869317804477026</v>
       </c>
       <c r="M41" t="n">
         <v>0.16839886741129</v>
@@ -3607,13 +3607,13 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s">
         <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D42" t="s">
         <v>25</v>
@@ -3664,18 +3664,18 @@
         <v>0.855072463768116</v>
       </c>
       <c r="T42" t="n">
-        <v>0.905797101449275</v>
+        <v>0.978260869565217</v>
       </c>
       <c r="U42" t="n">
         <v>0.710144927536232</v>
       </c>
       <c r="V42" t="n">
-        <v>0.720496894409938</v>
+        <v>0.730848861283644</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B43" t="s">
         <v>23</v>
@@ -3732,18 +3732,18 @@
         <v>0.710144927536232</v>
       </c>
       <c r="T43" t="n">
-        <v>0.710144927536232</v>
+        <v>0.739130434782609</v>
       </c>
       <c r="U43" t="n">
         <v>0.826086956521739</v>
       </c>
       <c r="V43" t="n">
-        <v>0.752587991718426</v>
+        <v>0.756728778467909</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B44" t="s">
         <v>23</v>
@@ -3811,7 +3811,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B45" t="s">
         <v>23</v>
@@ -3826,7 +3826,7 @@
         <v>56</v>
       </c>
       <c r="F45" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="G45" t="n">
         <v>11</v>
@@ -3844,7 +3844,7 @@
         <v>0.00862732481383353</v>
       </c>
       <c r="L45" t="n">
-        <v>0.0869113264453914</v>
+        <v>0.0869113264453916</v>
       </c>
       <c r="M45" t="n">
         <v>0.17601299353614</v>
@@ -3879,7 +3879,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B46" t="s">
         <v>23</v>
@@ -3894,7 +3894,7 @@
         <v>31</v>
       </c>
       <c r="F46" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G46" t="n">
         <v>9</v>
@@ -3947,13 +3947,13 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B47" t="s">
         <v>23</v>
       </c>
       <c r="C47" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D47" t="s">
         <v>25</v>
@@ -3980,7 +3980,7 @@
         <v>0.00845880699654408</v>
       </c>
       <c r="L47" t="n">
-        <v>0.0583970592156716</v>
+        <v>0.0583970592156718</v>
       </c>
       <c r="M47" t="n">
         <v>0.417432720158376</v>
@@ -4015,13 +4015,13 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B48" t="s">
         <v>23</v>
       </c>
       <c r="C48" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D48" t="s">
         <v>91</v>
@@ -4048,7 +4048,7 @@
         <v>0.00622689957285076</v>
       </c>
       <c r="L48" t="n">
-        <v>0.0354861648513936</v>
+        <v>0.0354861648513937</v>
       </c>
       <c r="M48" t="n">
         <v>0.255583152242378</v>
@@ -4083,7 +4083,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
         <v>47</v>
@@ -4098,7 +4098,7 @@
         <v>56</v>
       </c>
       <c r="F49" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="G49" t="n">
         <v>18</v>
@@ -4116,7 +4116,7 @@
         <v>0.0128582660620001</v>
       </c>
       <c r="L49" t="n">
-        <v>0.094939924301289</v>
+        <v>0.0949399243012892</v>
       </c>
       <c r="M49" t="n">
         <v>0.14970877234968</v>
@@ -4151,7 +4151,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B50" t="s">
         <v>23</v>
@@ -4208,18 +4208,18 @@
         <v>0.652173913043478</v>
       </c>
       <c r="T50" t="n">
-        <v>0.449275362318841</v>
+        <v>0.420289855072464</v>
       </c>
       <c r="U50" t="n">
         <v>0.318840579710145</v>
       </c>
       <c r="V50" t="n">
-        <v>0.472049689440994</v>
+        <v>0.467908902691511</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B51" t="s">
         <v>47</v>
@@ -4276,18 +4276,18 @@
         <v>0.594202898550725</v>
       </c>
       <c r="T51" t="n">
-        <v>0.449275362318841</v>
+        <v>0.442028985507246</v>
       </c>
       <c r="U51" t="n">
         <v>0.318840579710145</v>
       </c>
       <c r="V51" t="n">
-        <v>0.463768115942029</v>
+        <v>0.462732919254658</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B52" t="s">
         <v>23</v>
@@ -4344,18 +4344,18 @@
         <v>0.985507246376812</v>
       </c>
       <c r="T52" t="n">
-        <v>0.86231884057971</v>
+        <v>0.855072463768116</v>
       </c>
       <c r="U52" t="n">
         <v>0.992753623188406</v>
       </c>
       <c r="V52" t="n">
-        <v>0.973084886128364</v>
+        <v>0.972049689440994</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B53" t="s">
         <v>23</v>
@@ -4423,7 +4423,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B54" t="s">
         <v>23</v>
@@ -4480,18 +4480,18 @@
         <v>0.855072463768116</v>
       </c>
       <c r="T54" t="n">
-        <v>0.992753623188406</v>
+        <v>0.978260869565217</v>
       </c>
       <c r="U54" t="n">
         <v>0.710144927536232</v>
       </c>
       <c r="V54" t="n">
-        <v>0.732919254658385</v>
+        <v>0.730848861283644</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B55" t="s">
         <v>47</v>
@@ -4506,7 +4506,7 @@
         <v>88</v>
       </c>
       <c r="F55" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="G55" t="n">
         <v>10</v>
@@ -4524,7 +4524,7 @@
         <v>0.00850422082582812</v>
       </c>
       <c r="L55" t="n">
-        <v>0.0515376807914378</v>
+        <v>0.051537680791438</v>
       </c>
       <c r="M55" t="n">
         <v>0.206794003121212</v>
@@ -4660,7 +4660,7 @@
         <v>0.0127746107900135</v>
       </c>
       <c r="L57" t="n">
-        <v>0.0789752608604363</v>
+        <v>0.0789752608604366</v>
       </c>
       <c r="M57" t="n">
         <v>0.182396400643084</v>
@@ -4752,13 +4752,13 @@
         <v>0.905797101449275</v>
       </c>
       <c r="T58" t="n">
-        <v>0.949275362318841</v>
+        <v>0.978260869565217</v>
       </c>
       <c r="U58" t="n">
         <v>0.710144927536232</v>
       </c>
       <c r="V58" t="n">
-        <v>0.733954451345756</v>
+        <v>0.738095238095238</v>
       </c>
     </row>
     <row r="59">
@@ -4820,13 +4820,13 @@
         <v>0.623188405797101</v>
       </c>
       <c r="T59" t="n">
-        <v>0.485507246376812</v>
+        <v>0.478260869565217</v>
       </c>
       <c r="U59" t="n">
         <v>0.36231884057971</v>
       </c>
       <c r="V59" t="n">
-        <v>0.479296066252588</v>
+        <v>0.478260869565217</v>
       </c>
     </row>
     <row r="60">
@@ -4888,13 +4888,13 @@
         <v>0.623188405797101</v>
       </c>
       <c r="T60" t="n">
-        <v>0.485507246376812</v>
+        <v>0.492753623188406</v>
       </c>
       <c r="U60" t="n">
         <v>0.36231884057971</v>
       </c>
       <c r="V60" t="n">
-        <v>0.479296066252588</v>
+        <v>0.480331262939959</v>
       </c>
     </row>
     <row r="61">
@@ -4932,7 +4932,7 @@
         <v>0.0170732846261839</v>
       </c>
       <c r="L61" t="n">
-        <v>0.190997599320271</v>
+        <v>0.190997599320272</v>
       </c>
       <c r="M61" t="n">
         <v>0.167341457993028</v>
@@ -4956,13 +4956,13 @@
         <v>0.623188405797101</v>
       </c>
       <c r="T61" t="n">
-        <v>0.449275362318841</v>
+        <v>0.463768115942029</v>
       </c>
       <c r="U61" t="n">
         <v>0.36231884057971</v>
       </c>
       <c r="V61" t="n">
-        <v>0.474120082815735</v>
+        <v>0.476190476190476</v>
       </c>
     </row>
     <row r="62">
@@ -5092,13 +5092,13 @@
         <v>0.855072463768116</v>
       </c>
       <c r="T63" t="n">
-        <v>0.992753623188406</v>
+        <v>0.91304347826087</v>
       </c>
       <c r="U63" t="n">
         <v>0.710144927536232</v>
       </c>
       <c r="V63" t="n">
-        <v>0.732919254658385</v>
+        <v>0.721532091097308</v>
       </c>
     </row>
     <row r="64">
@@ -5160,13 +5160,13 @@
         <v>0.905797101449275</v>
       </c>
       <c r="T64" t="n">
-        <v>0.949275362318841</v>
+        <v>0.91304347826087</v>
       </c>
       <c r="U64" t="n">
         <v>0.710144927536232</v>
       </c>
       <c r="V64" t="n">
-        <v>0.733954451345756</v>
+        <v>0.728778467908903</v>
       </c>
     </row>
     <row r="65">
@@ -5228,13 +5228,13 @@
         <v>0.688405797101449</v>
       </c>
       <c r="T65" t="n">
-        <v>0.72463768115942</v>
+        <v>0.710144927536232</v>
       </c>
       <c r="U65" t="n">
         <v>0.804347826086957</v>
       </c>
       <c r="V65" t="n">
-        <v>0.748447204968944</v>
+        <v>0.746376811594203</v>
       </c>
     </row>
     <row r="66">
@@ -5254,7 +5254,7 @@
         <v>31</v>
       </c>
       <c r="F66" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="G66" t="n">
         <v>12</v>
@@ -5272,7 +5272,7 @@
         <v>0.0100704564135229</v>
       </c>
       <c r="L66" t="n">
-        <v>0.058301105556326</v>
+        <v>0.0583011055563262</v>
       </c>
       <c r="M66" t="n">
         <v>0.176168786295844</v>
@@ -5364,13 +5364,13 @@
         <v>1</v>
       </c>
       <c r="T67" t="n">
-        <v>0.86231884057971</v>
+        <v>0.869565217391304</v>
       </c>
       <c r="U67" t="n">
         <v>0.992753623188406</v>
       </c>
       <c r="V67" t="n">
-        <v>0.975155279503106</v>
+        <v>0.976190476190476</v>
       </c>
     </row>
     <row r="68">
@@ -5432,13 +5432,13 @@
         <v>0.688405797101449</v>
       </c>
       <c r="T68" t="n">
-        <v>0.739130434782609</v>
+        <v>0.72463768115942</v>
       </c>
       <c r="U68" t="n">
         <v>0.804347826086957</v>
       </c>
       <c r="V68" t="n">
-        <v>0.750517598343685</v>
+        <v>0.748447204968944</v>
       </c>
     </row>
     <row r="69">
@@ -5500,13 +5500,13 @@
         <v>0.579710144927536</v>
       </c>
       <c r="T69" t="n">
-        <v>0.826086956521739</v>
+        <v>0.811594202898551</v>
       </c>
       <c r="U69" t="n">
         <v>0.608695652173913</v>
       </c>
       <c r="V69" t="n">
-        <v>0.63871635610766</v>
+        <v>0.636645962732919</v>
       </c>
     </row>
     <row r="70">
@@ -5544,7 +5544,7 @@
         <v>0.0179163651293508</v>
       </c>
       <c r="L70" t="n">
-        <v>0.74086376869859</v>
+        <v>0.740863768698589</v>
       </c>
       <c r="M70" t="n">
         <v>0.107241990427333</v>
@@ -5610,13 +5610,13 @@
         <v>27</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>0.161835748792271</v>
+        <v>0.0885093167701863</v>
       </c>
     </row>
     <row r="3">
@@ -5624,27 +5624,27 @@
         <v>94</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.268115942028985</v>
+        <v>0.202898550724638</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>0.188405797101449</v>
+        <v>0.301863354037267</v>
       </c>
     </row>
     <row r="5">
@@ -5694,13 +5694,13 @@
         <v>43</v>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0.158385093167702</v>
+        <v>0.0807453416149068</v>
       </c>
     </row>
     <row r="9">
@@ -5722,13 +5722,13 @@
         <v>71</v>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>0.279761904761905</v>
+        <v>0.139751552795031</v>
       </c>
     </row>
     <row r="11">
@@ -5736,13 +5736,13 @@
         <v>73</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11" t="n">
-        <v>0.160455486542443</v>
+        <v>0.20703933747412</v>
       </c>
     </row>
     <row r="12">
@@ -5753,10 +5753,10 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.317287784679089</v>
+        <v>0.38768115942029</v>
       </c>
     </row>
   </sheetData>

</xml_diff>